<commit_message>
Updated motor model using in-house regression
</commit_message>
<xml_diff>
--- a/data/motors/motor_data.xlsx
+++ b/data/motors/motor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/data/motors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3ADBCF-19BC-A643-BB2A-15A7EA9CE4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9A4989-DE07-6447-8781-2C535F7A4524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17120" activeTab="1" xr2:uid="{2F87124F-FADD-1C4B-8E1F-F5E2F237BAFB}"/>
   </bookViews>
@@ -8973,6 +8973,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -23093,8 +23094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EA9C6B-7942-C84D-BA2E-598934CE2C8D}">
   <dimension ref="B2:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="91" workbookViewId="0">
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>